<commit_message>
reflex agent with internal state
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="6">
   <si>
     <t xml:space="preserve">environment</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dirty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clean</t>
   </si>
 </sst>
 </file>
@@ -137,11 +140,11 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -195,7 +198,9 @@
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -207,7 +212,9 @@
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -216,7 +223,9 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
@@ -228,7 +237,9 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
@@ -240,8 +251,12 @@
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -250,8 +265,12 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>